<commit_message>
Added additional Papaya SRA projects
</commit_message>
<xml_diff>
--- a/data/Cpapaya_PRJNA727683_sra_wgs.xlsx
+++ b/data/Cpapaya_PRJNA727683_sra_wgs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griffitheduau.sharepoint.com/sites/PapayaFlavour9/Shared Documents/Research Projects/Leela_PhD_Papaya_Genomics/Thesis/GWAS/SNP_Calling_Papaya/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{6217C796-E37C-47A2-BAF7-E5C73618BCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F7A9796-D418-4809-8169-9BE7242B8B60}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="8_{6217C796-E37C-47A2-BAF7-E5C73618BCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09836BC2-6EA9-4C68-B8DA-425FE49C920E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{747801C4-3124-4AAF-9AC0-4E8FC5249F5F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{747801C4-3124-4AAF-9AC0-4E8FC5249F5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Cpapaya_PRJNA727683_sra_wgs" sheetId="1" r:id="rId1"/>
@@ -2284,10 +2284,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{760FFDF1-3656-4DAE-B871-4D76DAD459C6}" name="Table2" displayName="Table2" ref="A1:R89" totalsRowShown="0">
   <autoFilter ref="A1:R89" xr:uid="{760FFDF1-3656-4DAE-B871-4D76DAD459C6}"/>
@@ -2651,27 +2647,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7FCFC9-6A17-4D9F-B5ED-EB51F23802FD}">
   <dimension ref="A1:R89"/>
   <sheetViews>
-    <sheetView topLeftCell="C49" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J62" sqref="J62"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" customWidth="1"/>
-    <col min="12" max="13" width="12.5703125" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" customWidth="1"/>
-    <col min="15" max="15" width="16.5703125" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" customWidth="1"/>
-    <col min="17" max="17" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
+    <col min="2" max="3" width="16.54296875" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" customWidth="1"/>
+    <col min="9" max="9" width="13.54296875" customWidth="1"/>
+    <col min="10" max="10" width="14.81640625" customWidth="1"/>
+    <col min="11" max="11" width="22.453125" customWidth="1"/>
+    <col min="12" max="13" width="12.54296875" customWidth="1"/>
+    <col min="14" max="14" width="14.453125" customWidth="1"/>
+    <col min="15" max="15" width="16.54296875" customWidth="1"/>
+    <col min="16" max="16" width="15.453125" customWidth="1"/>
+    <col min="17" max="17" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -7758,336 +7754,336 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A71EFF89-66B7-4C88-B6F3-2616DBE242AE}">
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" style="1" customWidth="1"/>
     <col min="6" max="256" width="10" style="1"/>
-    <col min="257" max="257" width="16.140625" style="1" customWidth="1"/>
+    <col min="257" max="257" width="16.1796875" style="1" customWidth="1"/>
     <col min="258" max="259" width="10" style="1"/>
-    <col min="260" max="260" width="14.42578125" style="1" customWidth="1"/>
-    <col min="261" max="261" width="13.42578125" style="1" customWidth="1"/>
+    <col min="260" max="260" width="14.453125" style="1" customWidth="1"/>
+    <col min="261" max="261" width="13.453125" style="1" customWidth="1"/>
     <col min="262" max="512" width="10" style="1"/>
-    <col min="513" max="513" width="16.140625" style="1" customWidth="1"/>
+    <col min="513" max="513" width="16.1796875" style="1" customWidth="1"/>
     <col min="514" max="515" width="10" style="1"/>
-    <col min="516" max="516" width="14.42578125" style="1" customWidth="1"/>
-    <col min="517" max="517" width="13.42578125" style="1" customWidth="1"/>
+    <col min="516" max="516" width="14.453125" style="1" customWidth="1"/>
+    <col min="517" max="517" width="13.453125" style="1" customWidth="1"/>
     <col min="518" max="768" width="10" style="1"/>
-    <col min="769" max="769" width="16.140625" style="1" customWidth="1"/>
+    <col min="769" max="769" width="16.1796875" style="1" customWidth="1"/>
     <col min="770" max="771" width="10" style="1"/>
-    <col min="772" max="772" width="14.42578125" style="1" customWidth="1"/>
-    <col min="773" max="773" width="13.42578125" style="1" customWidth="1"/>
+    <col min="772" max="772" width="14.453125" style="1" customWidth="1"/>
+    <col min="773" max="773" width="13.453125" style="1" customWidth="1"/>
     <col min="774" max="1024" width="10" style="1"/>
-    <col min="1025" max="1025" width="16.140625" style="1" customWidth="1"/>
+    <col min="1025" max="1025" width="16.1796875" style="1" customWidth="1"/>
     <col min="1026" max="1027" width="10" style="1"/>
-    <col min="1028" max="1028" width="14.42578125" style="1" customWidth="1"/>
-    <col min="1029" max="1029" width="13.42578125" style="1" customWidth="1"/>
+    <col min="1028" max="1028" width="14.453125" style="1" customWidth="1"/>
+    <col min="1029" max="1029" width="13.453125" style="1" customWidth="1"/>
     <col min="1030" max="1280" width="10" style="1"/>
-    <col min="1281" max="1281" width="16.140625" style="1" customWidth="1"/>
+    <col min="1281" max="1281" width="16.1796875" style="1" customWidth="1"/>
     <col min="1282" max="1283" width="10" style="1"/>
-    <col min="1284" max="1284" width="14.42578125" style="1" customWidth="1"/>
-    <col min="1285" max="1285" width="13.42578125" style="1" customWidth="1"/>
+    <col min="1284" max="1284" width="14.453125" style="1" customWidth="1"/>
+    <col min="1285" max="1285" width="13.453125" style="1" customWidth="1"/>
     <col min="1286" max="1536" width="10" style="1"/>
-    <col min="1537" max="1537" width="16.140625" style="1" customWidth="1"/>
+    <col min="1537" max="1537" width="16.1796875" style="1" customWidth="1"/>
     <col min="1538" max="1539" width="10" style="1"/>
-    <col min="1540" max="1540" width="14.42578125" style="1" customWidth="1"/>
-    <col min="1541" max="1541" width="13.42578125" style="1" customWidth="1"/>
+    <col min="1540" max="1540" width="14.453125" style="1" customWidth="1"/>
+    <col min="1541" max="1541" width="13.453125" style="1" customWidth="1"/>
     <col min="1542" max="1792" width="10" style="1"/>
-    <col min="1793" max="1793" width="16.140625" style="1" customWidth="1"/>
+    <col min="1793" max="1793" width="16.1796875" style="1" customWidth="1"/>
     <col min="1794" max="1795" width="10" style="1"/>
-    <col min="1796" max="1796" width="14.42578125" style="1" customWidth="1"/>
-    <col min="1797" max="1797" width="13.42578125" style="1" customWidth="1"/>
+    <col min="1796" max="1796" width="14.453125" style="1" customWidth="1"/>
+    <col min="1797" max="1797" width="13.453125" style="1" customWidth="1"/>
     <col min="1798" max="2048" width="10" style="1"/>
-    <col min="2049" max="2049" width="16.140625" style="1" customWidth="1"/>
+    <col min="2049" max="2049" width="16.1796875" style="1" customWidth="1"/>
     <col min="2050" max="2051" width="10" style="1"/>
-    <col min="2052" max="2052" width="14.42578125" style="1" customWidth="1"/>
-    <col min="2053" max="2053" width="13.42578125" style="1" customWidth="1"/>
+    <col min="2052" max="2052" width="14.453125" style="1" customWidth="1"/>
+    <col min="2053" max="2053" width="13.453125" style="1" customWidth="1"/>
     <col min="2054" max="2304" width="10" style="1"/>
-    <col min="2305" max="2305" width="16.140625" style="1" customWidth="1"/>
+    <col min="2305" max="2305" width="16.1796875" style="1" customWidth="1"/>
     <col min="2306" max="2307" width="10" style="1"/>
-    <col min="2308" max="2308" width="14.42578125" style="1" customWidth="1"/>
-    <col min="2309" max="2309" width="13.42578125" style="1" customWidth="1"/>
+    <col min="2308" max="2308" width="14.453125" style="1" customWidth="1"/>
+    <col min="2309" max="2309" width="13.453125" style="1" customWidth="1"/>
     <col min="2310" max="2560" width="10" style="1"/>
-    <col min="2561" max="2561" width="16.140625" style="1" customWidth="1"/>
+    <col min="2561" max="2561" width="16.1796875" style="1" customWidth="1"/>
     <col min="2562" max="2563" width="10" style="1"/>
-    <col min="2564" max="2564" width="14.42578125" style="1" customWidth="1"/>
-    <col min="2565" max="2565" width="13.42578125" style="1" customWidth="1"/>
+    <col min="2564" max="2564" width="14.453125" style="1" customWidth="1"/>
+    <col min="2565" max="2565" width="13.453125" style="1" customWidth="1"/>
     <col min="2566" max="2816" width="10" style="1"/>
-    <col min="2817" max="2817" width="16.140625" style="1" customWidth="1"/>
+    <col min="2817" max="2817" width="16.1796875" style="1" customWidth="1"/>
     <col min="2818" max="2819" width="10" style="1"/>
-    <col min="2820" max="2820" width="14.42578125" style="1" customWidth="1"/>
-    <col min="2821" max="2821" width="13.42578125" style="1" customWidth="1"/>
+    <col min="2820" max="2820" width="14.453125" style="1" customWidth="1"/>
+    <col min="2821" max="2821" width="13.453125" style="1" customWidth="1"/>
     <col min="2822" max="3072" width="10" style="1"/>
-    <col min="3073" max="3073" width="16.140625" style="1" customWidth="1"/>
+    <col min="3073" max="3073" width="16.1796875" style="1" customWidth="1"/>
     <col min="3074" max="3075" width="10" style="1"/>
-    <col min="3076" max="3076" width="14.42578125" style="1" customWidth="1"/>
-    <col min="3077" max="3077" width="13.42578125" style="1" customWidth="1"/>
+    <col min="3076" max="3076" width="14.453125" style="1" customWidth="1"/>
+    <col min="3077" max="3077" width="13.453125" style="1" customWidth="1"/>
     <col min="3078" max="3328" width="10" style="1"/>
-    <col min="3329" max="3329" width="16.140625" style="1" customWidth="1"/>
+    <col min="3329" max="3329" width="16.1796875" style="1" customWidth="1"/>
     <col min="3330" max="3331" width="10" style="1"/>
-    <col min="3332" max="3332" width="14.42578125" style="1" customWidth="1"/>
-    <col min="3333" max="3333" width="13.42578125" style="1" customWidth="1"/>
+    <col min="3332" max="3332" width="14.453125" style="1" customWidth="1"/>
+    <col min="3333" max="3333" width="13.453125" style="1" customWidth="1"/>
     <col min="3334" max="3584" width="10" style="1"/>
-    <col min="3585" max="3585" width="16.140625" style="1" customWidth="1"/>
+    <col min="3585" max="3585" width="16.1796875" style="1" customWidth="1"/>
     <col min="3586" max="3587" width="10" style="1"/>
-    <col min="3588" max="3588" width="14.42578125" style="1" customWidth="1"/>
-    <col min="3589" max="3589" width="13.42578125" style="1" customWidth="1"/>
+    <col min="3588" max="3588" width="14.453125" style="1" customWidth="1"/>
+    <col min="3589" max="3589" width="13.453125" style="1" customWidth="1"/>
     <col min="3590" max="3840" width="10" style="1"/>
-    <col min="3841" max="3841" width="16.140625" style="1" customWidth="1"/>
+    <col min="3841" max="3841" width="16.1796875" style="1" customWidth="1"/>
     <col min="3842" max="3843" width="10" style="1"/>
-    <col min="3844" max="3844" width="14.42578125" style="1" customWidth="1"/>
-    <col min="3845" max="3845" width="13.42578125" style="1" customWidth="1"/>
+    <col min="3844" max="3844" width="14.453125" style="1" customWidth="1"/>
+    <col min="3845" max="3845" width="13.453125" style="1" customWidth="1"/>
     <col min="3846" max="4096" width="10" style="1"/>
-    <col min="4097" max="4097" width="16.140625" style="1" customWidth="1"/>
+    <col min="4097" max="4097" width="16.1796875" style="1" customWidth="1"/>
     <col min="4098" max="4099" width="10" style="1"/>
-    <col min="4100" max="4100" width="14.42578125" style="1" customWidth="1"/>
-    <col min="4101" max="4101" width="13.42578125" style="1" customWidth="1"/>
+    <col min="4100" max="4100" width="14.453125" style="1" customWidth="1"/>
+    <col min="4101" max="4101" width="13.453125" style="1" customWidth="1"/>
     <col min="4102" max="4352" width="10" style="1"/>
-    <col min="4353" max="4353" width="16.140625" style="1" customWidth="1"/>
+    <col min="4353" max="4353" width="16.1796875" style="1" customWidth="1"/>
     <col min="4354" max="4355" width="10" style="1"/>
-    <col min="4356" max="4356" width="14.42578125" style="1" customWidth="1"/>
-    <col min="4357" max="4357" width="13.42578125" style="1" customWidth="1"/>
+    <col min="4356" max="4356" width="14.453125" style="1" customWidth="1"/>
+    <col min="4357" max="4357" width="13.453125" style="1" customWidth="1"/>
     <col min="4358" max="4608" width="10" style="1"/>
-    <col min="4609" max="4609" width="16.140625" style="1" customWidth="1"/>
+    <col min="4609" max="4609" width="16.1796875" style="1" customWidth="1"/>
     <col min="4610" max="4611" width="10" style="1"/>
-    <col min="4612" max="4612" width="14.42578125" style="1" customWidth="1"/>
-    <col min="4613" max="4613" width="13.42578125" style="1" customWidth="1"/>
+    <col min="4612" max="4612" width="14.453125" style="1" customWidth="1"/>
+    <col min="4613" max="4613" width="13.453125" style="1" customWidth="1"/>
     <col min="4614" max="4864" width="10" style="1"/>
-    <col min="4865" max="4865" width="16.140625" style="1" customWidth="1"/>
+    <col min="4865" max="4865" width="16.1796875" style="1" customWidth="1"/>
     <col min="4866" max="4867" width="10" style="1"/>
-    <col min="4868" max="4868" width="14.42578125" style="1" customWidth="1"/>
-    <col min="4869" max="4869" width="13.42578125" style="1" customWidth="1"/>
+    <col min="4868" max="4868" width="14.453125" style="1" customWidth="1"/>
+    <col min="4869" max="4869" width="13.453125" style="1" customWidth="1"/>
     <col min="4870" max="5120" width="10" style="1"/>
-    <col min="5121" max="5121" width="16.140625" style="1" customWidth="1"/>
+    <col min="5121" max="5121" width="16.1796875" style="1" customWidth="1"/>
     <col min="5122" max="5123" width="10" style="1"/>
-    <col min="5124" max="5124" width="14.42578125" style="1" customWidth="1"/>
-    <col min="5125" max="5125" width="13.42578125" style="1" customWidth="1"/>
+    <col min="5124" max="5124" width="14.453125" style="1" customWidth="1"/>
+    <col min="5125" max="5125" width="13.453125" style="1" customWidth="1"/>
     <col min="5126" max="5376" width="10" style="1"/>
-    <col min="5377" max="5377" width="16.140625" style="1" customWidth="1"/>
+    <col min="5377" max="5377" width="16.1796875" style="1" customWidth="1"/>
     <col min="5378" max="5379" width="10" style="1"/>
-    <col min="5380" max="5380" width="14.42578125" style="1" customWidth="1"/>
-    <col min="5381" max="5381" width="13.42578125" style="1" customWidth="1"/>
+    <col min="5380" max="5380" width="14.453125" style="1" customWidth="1"/>
+    <col min="5381" max="5381" width="13.453125" style="1" customWidth="1"/>
     <col min="5382" max="5632" width="10" style="1"/>
-    <col min="5633" max="5633" width="16.140625" style="1" customWidth="1"/>
+    <col min="5633" max="5633" width="16.1796875" style="1" customWidth="1"/>
     <col min="5634" max="5635" width="10" style="1"/>
-    <col min="5636" max="5636" width="14.42578125" style="1" customWidth="1"/>
-    <col min="5637" max="5637" width="13.42578125" style="1" customWidth="1"/>
+    <col min="5636" max="5636" width="14.453125" style="1" customWidth="1"/>
+    <col min="5637" max="5637" width="13.453125" style="1" customWidth="1"/>
     <col min="5638" max="5888" width="10" style="1"/>
-    <col min="5889" max="5889" width="16.140625" style="1" customWidth="1"/>
+    <col min="5889" max="5889" width="16.1796875" style="1" customWidth="1"/>
     <col min="5890" max="5891" width="10" style="1"/>
-    <col min="5892" max="5892" width="14.42578125" style="1" customWidth="1"/>
-    <col min="5893" max="5893" width="13.42578125" style="1" customWidth="1"/>
+    <col min="5892" max="5892" width="14.453125" style="1" customWidth="1"/>
+    <col min="5893" max="5893" width="13.453125" style="1" customWidth="1"/>
     <col min="5894" max="6144" width="10" style="1"/>
-    <col min="6145" max="6145" width="16.140625" style="1" customWidth="1"/>
+    <col min="6145" max="6145" width="16.1796875" style="1" customWidth="1"/>
     <col min="6146" max="6147" width="10" style="1"/>
-    <col min="6148" max="6148" width="14.42578125" style="1" customWidth="1"/>
-    <col min="6149" max="6149" width="13.42578125" style="1" customWidth="1"/>
+    <col min="6148" max="6148" width="14.453125" style="1" customWidth="1"/>
+    <col min="6149" max="6149" width="13.453125" style="1" customWidth="1"/>
     <col min="6150" max="6400" width="10" style="1"/>
-    <col min="6401" max="6401" width="16.140625" style="1" customWidth="1"/>
+    <col min="6401" max="6401" width="16.1796875" style="1" customWidth="1"/>
     <col min="6402" max="6403" width="10" style="1"/>
-    <col min="6404" max="6404" width="14.42578125" style="1" customWidth="1"/>
-    <col min="6405" max="6405" width="13.42578125" style="1" customWidth="1"/>
+    <col min="6404" max="6404" width="14.453125" style="1" customWidth="1"/>
+    <col min="6405" max="6405" width="13.453125" style="1" customWidth="1"/>
     <col min="6406" max="6656" width="10" style="1"/>
-    <col min="6657" max="6657" width="16.140625" style="1" customWidth="1"/>
+    <col min="6657" max="6657" width="16.1796875" style="1" customWidth="1"/>
     <col min="6658" max="6659" width="10" style="1"/>
-    <col min="6660" max="6660" width="14.42578125" style="1" customWidth="1"/>
-    <col min="6661" max="6661" width="13.42578125" style="1" customWidth="1"/>
+    <col min="6660" max="6660" width="14.453125" style="1" customWidth="1"/>
+    <col min="6661" max="6661" width="13.453125" style="1" customWidth="1"/>
     <col min="6662" max="6912" width="10" style="1"/>
-    <col min="6913" max="6913" width="16.140625" style="1" customWidth="1"/>
+    <col min="6913" max="6913" width="16.1796875" style="1" customWidth="1"/>
     <col min="6914" max="6915" width="10" style="1"/>
-    <col min="6916" max="6916" width="14.42578125" style="1" customWidth="1"/>
-    <col min="6917" max="6917" width="13.42578125" style="1" customWidth="1"/>
+    <col min="6916" max="6916" width="14.453125" style="1" customWidth="1"/>
+    <col min="6917" max="6917" width="13.453125" style="1" customWidth="1"/>
     <col min="6918" max="7168" width="10" style="1"/>
-    <col min="7169" max="7169" width="16.140625" style="1" customWidth="1"/>
+    <col min="7169" max="7169" width="16.1796875" style="1" customWidth="1"/>
     <col min="7170" max="7171" width="10" style="1"/>
-    <col min="7172" max="7172" width="14.42578125" style="1" customWidth="1"/>
-    <col min="7173" max="7173" width="13.42578125" style="1" customWidth="1"/>
+    <col min="7172" max="7172" width="14.453125" style="1" customWidth="1"/>
+    <col min="7173" max="7173" width="13.453125" style="1" customWidth="1"/>
     <col min="7174" max="7424" width="10" style="1"/>
-    <col min="7425" max="7425" width="16.140625" style="1" customWidth="1"/>
+    <col min="7425" max="7425" width="16.1796875" style="1" customWidth="1"/>
     <col min="7426" max="7427" width="10" style="1"/>
-    <col min="7428" max="7428" width="14.42578125" style="1" customWidth="1"/>
-    <col min="7429" max="7429" width="13.42578125" style="1" customWidth="1"/>
+    <col min="7428" max="7428" width="14.453125" style="1" customWidth="1"/>
+    <col min="7429" max="7429" width="13.453125" style="1" customWidth="1"/>
     <col min="7430" max="7680" width="10" style="1"/>
-    <col min="7681" max="7681" width="16.140625" style="1" customWidth="1"/>
+    <col min="7681" max="7681" width="16.1796875" style="1" customWidth="1"/>
     <col min="7682" max="7683" width="10" style="1"/>
-    <col min="7684" max="7684" width="14.42578125" style="1" customWidth="1"/>
-    <col min="7685" max="7685" width="13.42578125" style="1" customWidth="1"/>
+    <col min="7684" max="7684" width="14.453125" style="1" customWidth="1"/>
+    <col min="7685" max="7685" width="13.453125" style="1" customWidth="1"/>
     <col min="7686" max="7936" width="10" style="1"/>
-    <col min="7937" max="7937" width="16.140625" style="1" customWidth="1"/>
+    <col min="7937" max="7937" width="16.1796875" style="1" customWidth="1"/>
     <col min="7938" max="7939" width="10" style="1"/>
-    <col min="7940" max="7940" width="14.42578125" style="1" customWidth="1"/>
-    <col min="7941" max="7941" width="13.42578125" style="1" customWidth="1"/>
+    <col min="7940" max="7940" width="14.453125" style="1" customWidth="1"/>
+    <col min="7941" max="7941" width="13.453125" style="1" customWidth="1"/>
     <col min="7942" max="8192" width="10" style="1"/>
-    <col min="8193" max="8193" width="16.140625" style="1" customWidth="1"/>
+    <col min="8193" max="8193" width="16.1796875" style="1" customWidth="1"/>
     <col min="8194" max="8195" width="10" style="1"/>
-    <col min="8196" max="8196" width="14.42578125" style="1" customWidth="1"/>
-    <col min="8197" max="8197" width="13.42578125" style="1" customWidth="1"/>
+    <col min="8196" max="8196" width="14.453125" style="1" customWidth="1"/>
+    <col min="8197" max="8197" width="13.453125" style="1" customWidth="1"/>
     <col min="8198" max="8448" width="10" style="1"/>
-    <col min="8449" max="8449" width="16.140625" style="1" customWidth="1"/>
+    <col min="8449" max="8449" width="16.1796875" style="1" customWidth="1"/>
     <col min="8450" max="8451" width="10" style="1"/>
-    <col min="8452" max="8452" width="14.42578125" style="1" customWidth="1"/>
-    <col min="8453" max="8453" width="13.42578125" style="1" customWidth="1"/>
+    <col min="8452" max="8452" width="14.453125" style="1" customWidth="1"/>
+    <col min="8453" max="8453" width="13.453125" style="1" customWidth="1"/>
     <col min="8454" max="8704" width="10" style="1"/>
-    <col min="8705" max="8705" width="16.140625" style="1" customWidth="1"/>
+    <col min="8705" max="8705" width="16.1796875" style="1" customWidth="1"/>
     <col min="8706" max="8707" width="10" style="1"/>
-    <col min="8708" max="8708" width="14.42578125" style="1" customWidth="1"/>
-    <col min="8709" max="8709" width="13.42578125" style="1" customWidth="1"/>
+    <col min="8708" max="8708" width="14.453125" style="1" customWidth="1"/>
+    <col min="8709" max="8709" width="13.453125" style="1" customWidth="1"/>
     <col min="8710" max="8960" width="10" style="1"/>
-    <col min="8961" max="8961" width="16.140625" style="1" customWidth="1"/>
+    <col min="8961" max="8961" width="16.1796875" style="1" customWidth="1"/>
     <col min="8962" max="8963" width="10" style="1"/>
-    <col min="8964" max="8964" width="14.42578125" style="1" customWidth="1"/>
-    <col min="8965" max="8965" width="13.42578125" style="1" customWidth="1"/>
+    <col min="8964" max="8964" width="14.453125" style="1" customWidth="1"/>
+    <col min="8965" max="8965" width="13.453125" style="1" customWidth="1"/>
     <col min="8966" max="9216" width="10" style="1"/>
-    <col min="9217" max="9217" width="16.140625" style="1" customWidth="1"/>
+    <col min="9217" max="9217" width="16.1796875" style="1" customWidth="1"/>
     <col min="9218" max="9219" width="10" style="1"/>
-    <col min="9220" max="9220" width="14.42578125" style="1" customWidth="1"/>
-    <col min="9221" max="9221" width="13.42578125" style="1" customWidth="1"/>
+    <col min="9220" max="9220" width="14.453125" style="1" customWidth="1"/>
+    <col min="9221" max="9221" width="13.453125" style="1" customWidth="1"/>
     <col min="9222" max="9472" width="10" style="1"/>
-    <col min="9473" max="9473" width="16.140625" style="1" customWidth="1"/>
+    <col min="9473" max="9473" width="16.1796875" style="1" customWidth="1"/>
     <col min="9474" max="9475" width="10" style="1"/>
-    <col min="9476" max="9476" width="14.42578125" style="1" customWidth="1"/>
-    <col min="9477" max="9477" width="13.42578125" style="1" customWidth="1"/>
+    <col min="9476" max="9476" width="14.453125" style="1" customWidth="1"/>
+    <col min="9477" max="9477" width="13.453125" style="1" customWidth="1"/>
     <col min="9478" max="9728" width="10" style="1"/>
-    <col min="9729" max="9729" width="16.140625" style="1" customWidth="1"/>
+    <col min="9729" max="9729" width="16.1796875" style="1" customWidth="1"/>
     <col min="9730" max="9731" width="10" style="1"/>
-    <col min="9732" max="9732" width="14.42578125" style="1" customWidth="1"/>
-    <col min="9733" max="9733" width="13.42578125" style="1" customWidth="1"/>
+    <col min="9732" max="9732" width="14.453125" style="1" customWidth="1"/>
+    <col min="9733" max="9733" width="13.453125" style="1" customWidth="1"/>
     <col min="9734" max="9984" width="10" style="1"/>
-    <col min="9985" max="9985" width="16.140625" style="1" customWidth="1"/>
+    <col min="9985" max="9985" width="16.1796875" style="1" customWidth="1"/>
     <col min="9986" max="9987" width="10" style="1"/>
-    <col min="9988" max="9988" width="14.42578125" style="1" customWidth="1"/>
-    <col min="9989" max="9989" width="13.42578125" style="1" customWidth="1"/>
+    <col min="9988" max="9988" width="14.453125" style="1" customWidth="1"/>
+    <col min="9989" max="9989" width="13.453125" style="1" customWidth="1"/>
     <col min="9990" max="10240" width="10" style="1"/>
-    <col min="10241" max="10241" width="16.140625" style="1" customWidth="1"/>
+    <col min="10241" max="10241" width="16.1796875" style="1" customWidth="1"/>
     <col min="10242" max="10243" width="10" style="1"/>
-    <col min="10244" max="10244" width="14.42578125" style="1" customWidth="1"/>
-    <col min="10245" max="10245" width="13.42578125" style="1" customWidth="1"/>
+    <col min="10244" max="10244" width="14.453125" style="1" customWidth="1"/>
+    <col min="10245" max="10245" width="13.453125" style="1" customWidth="1"/>
     <col min="10246" max="10496" width="10" style="1"/>
-    <col min="10497" max="10497" width="16.140625" style="1" customWidth="1"/>
+    <col min="10497" max="10497" width="16.1796875" style="1" customWidth="1"/>
     <col min="10498" max="10499" width="10" style="1"/>
-    <col min="10500" max="10500" width="14.42578125" style="1" customWidth="1"/>
-    <col min="10501" max="10501" width="13.42578125" style="1" customWidth="1"/>
+    <col min="10500" max="10500" width="14.453125" style="1" customWidth="1"/>
+    <col min="10501" max="10501" width="13.453125" style="1" customWidth="1"/>
     <col min="10502" max="10752" width="10" style="1"/>
-    <col min="10753" max="10753" width="16.140625" style="1" customWidth="1"/>
+    <col min="10753" max="10753" width="16.1796875" style="1" customWidth="1"/>
     <col min="10754" max="10755" width="10" style="1"/>
-    <col min="10756" max="10756" width="14.42578125" style="1" customWidth="1"/>
-    <col min="10757" max="10757" width="13.42578125" style="1" customWidth="1"/>
+    <col min="10756" max="10756" width="14.453125" style="1" customWidth="1"/>
+    <col min="10757" max="10757" width="13.453125" style="1" customWidth="1"/>
     <col min="10758" max="11008" width="10" style="1"/>
-    <col min="11009" max="11009" width="16.140625" style="1" customWidth="1"/>
+    <col min="11009" max="11009" width="16.1796875" style="1" customWidth="1"/>
     <col min="11010" max="11011" width="10" style="1"/>
-    <col min="11012" max="11012" width="14.42578125" style="1" customWidth="1"/>
-    <col min="11013" max="11013" width="13.42578125" style="1" customWidth="1"/>
+    <col min="11012" max="11012" width="14.453125" style="1" customWidth="1"/>
+    <col min="11013" max="11013" width="13.453125" style="1" customWidth="1"/>
     <col min="11014" max="11264" width="10" style="1"/>
-    <col min="11265" max="11265" width="16.140625" style="1" customWidth="1"/>
+    <col min="11265" max="11265" width="16.1796875" style="1" customWidth="1"/>
     <col min="11266" max="11267" width="10" style="1"/>
-    <col min="11268" max="11268" width="14.42578125" style="1" customWidth="1"/>
-    <col min="11269" max="11269" width="13.42578125" style="1" customWidth="1"/>
+    <col min="11268" max="11268" width="14.453125" style="1" customWidth="1"/>
+    <col min="11269" max="11269" width="13.453125" style="1" customWidth="1"/>
     <col min="11270" max="11520" width="10" style="1"/>
-    <col min="11521" max="11521" width="16.140625" style="1" customWidth="1"/>
+    <col min="11521" max="11521" width="16.1796875" style="1" customWidth="1"/>
     <col min="11522" max="11523" width="10" style="1"/>
-    <col min="11524" max="11524" width="14.42578125" style="1" customWidth="1"/>
-    <col min="11525" max="11525" width="13.42578125" style="1" customWidth="1"/>
+    <col min="11524" max="11524" width="14.453125" style="1" customWidth="1"/>
+    <col min="11525" max="11525" width="13.453125" style="1" customWidth="1"/>
     <col min="11526" max="11776" width="10" style="1"/>
-    <col min="11777" max="11777" width="16.140625" style="1" customWidth="1"/>
+    <col min="11777" max="11777" width="16.1796875" style="1" customWidth="1"/>
     <col min="11778" max="11779" width="10" style="1"/>
-    <col min="11780" max="11780" width="14.42578125" style="1" customWidth="1"/>
-    <col min="11781" max="11781" width="13.42578125" style="1" customWidth="1"/>
+    <col min="11780" max="11780" width="14.453125" style="1" customWidth="1"/>
+    <col min="11781" max="11781" width="13.453125" style="1" customWidth="1"/>
     <col min="11782" max="12032" width="10" style="1"/>
-    <col min="12033" max="12033" width="16.140625" style="1" customWidth="1"/>
+    <col min="12033" max="12033" width="16.1796875" style="1" customWidth="1"/>
     <col min="12034" max="12035" width="10" style="1"/>
-    <col min="12036" max="12036" width="14.42578125" style="1" customWidth="1"/>
-    <col min="12037" max="12037" width="13.42578125" style="1" customWidth="1"/>
+    <col min="12036" max="12036" width="14.453125" style="1" customWidth="1"/>
+    <col min="12037" max="12037" width="13.453125" style="1" customWidth="1"/>
     <col min="12038" max="12288" width="10" style="1"/>
-    <col min="12289" max="12289" width="16.140625" style="1" customWidth="1"/>
+    <col min="12289" max="12289" width="16.1796875" style="1" customWidth="1"/>
     <col min="12290" max="12291" width="10" style="1"/>
-    <col min="12292" max="12292" width="14.42578125" style="1" customWidth="1"/>
-    <col min="12293" max="12293" width="13.42578125" style="1" customWidth="1"/>
+    <col min="12292" max="12292" width="14.453125" style="1" customWidth="1"/>
+    <col min="12293" max="12293" width="13.453125" style="1" customWidth="1"/>
     <col min="12294" max="12544" width="10" style="1"/>
-    <col min="12545" max="12545" width="16.140625" style="1" customWidth="1"/>
+    <col min="12545" max="12545" width="16.1796875" style="1" customWidth="1"/>
     <col min="12546" max="12547" width="10" style="1"/>
-    <col min="12548" max="12548" width="14.42578125" style="1" customWidth="1"/>
-    <col min="12549" max="12549" width="13.42578125" style="1" customWidth="1"/>
+    <col min="12548" max="12548" width="14.453125" style="1" customWidth="1"/>
+    <col min="12549" max="12549" width="13.453125" style="1" customWidth="1"/>
     <col min="12550" max="12800" width="10" style="1"/>
-    <col min="12801" max="12801" width="16.140625" style="1" customWidth="1"/>
+    <col min="12801" max="12801" width="16.1796875" style="1" customWidth="1"/>
     <col min="12802" max="12803" width="10" style="1"/>
-    <col min="12804" max="12804" width="14.42578125" style="1" customWidth="1"/>
-    <col min="12805" max="12805" width="13.42578125" style="1" customWidth="1"/>
+    <col min="12804" max="12804" width="14.453125" style="1" customWidth="1"/>
+    <col min="12805" max="12805" width="13.453125" style="1" customWidth="1"/>
     <col min="12806" max="13056" width="10" style="1"/>
-    <col min="13057" max="13057" width="16.140625" style="1" customWidth="1"/>
+    <col min="13057" max="13057" width="16.1796875" style="1" customWidth="1"/>
     <col min="13058" max="13059" width="10" style="1"/>
-    <col min="13060" max="13060" width="14.42578125" style="1" customWidth="1"/>
-    <col min="13061" max="13061" width="13.42578125" style="1" customWidth="1"/>
+    <col min="13060" max="13060" width="14.453125" style="1" customWidth="1"/>
+    <col min="13061" max="13061" width="13.453125" style="1" customWidth="1"/>
     <col min="13062" max="13312" width="10" style="1"/>
-    <col min="13313" max="13313" width="16.140625" style="1" customWidth="1"/>
+    <col min="13313" max="13313" width="16.1796875" style="1" customWidth="1"/>
     <col min="13314" max="13315" width="10" style="1"/>
-    <col min="13316" max="13316" width="14.42578125" style="1" customWidth="1"/>
-    <col min="13317" max="13317" width="13.42578125" style="1" customWidth="1"/>
+    <col min="13316" max="13316" width="14.453125" style="1" customWidth="1"/>
+    <col min="13317" max="13317" width="13.453125" style="1" customWidth="1"/>
     <col min="13318" max="13568" width="10" style="1"/>
-    <col min="13569" max="13569" width="16.140625" style="1" customWidth="1"/>
+    <col min="13569" max="13569" width="16.1796875" style="1" customWidth="1"/>
     <col min="13570" max="13571" width="10" style="1"/>
-    <col min="13572" max="13572" width="14.42578125" style="1" customWidth="1"/>
-    <col min="13573" max="13573" width="13.42578125" style="1" customWidth="1"/>
+    <col min="13572" max="13572" width="14.453125" style="1" customWidth="1"/>
+    <col min="13573" max="13573" width="13.453125" style="1" customWidth="1"/>
     <col min="13574" max="13824" width="10" style="1"/>
-    <col min="13825" max="13825" width="16.140625" style="1" customWidth="1"/>
+    <col min="13825" max="13825" width="16.1796875" style="1" customWidth="1"/>
     <col min="13826" max="13827" width="10" style="1"/>
-    <col min="13828" max="13828" width="14.42578125" style="1" customWidth="1"/>
-    <col min="13829" max="13829" width="13.42578125" style="1" customWidth="1"/>
+    <col min="13828" max="13828" width="14.453125" style="1" customWidth="1"/>
+    <col min="13829" max="13829" width="13.453125" style="1" customWidth="1"/>
     <col min="13830" max="14080" width="10" style="1"/>
-    <col min="14081" max="14081" width="16.140625" style="1" customWidth="1"/>
+    <col min="14081" max="14081" width="16.1796875" style="1" customWidth="1"/>
     <col min="14082" max="14083" width="10" style="1"/>
-    <col min="14084" max="14084" width="14.42578125" style="1" customWidth="1"/>
-    <col min="14085" max="14085" width="13.42578125" style="1" customWidth="1"/>
+    <col min="14084" max="14084" width="14.453125" style="1" customWidth="1"/>
+    <col min="14085" max="14085" width="13.453125" style="1" customWidth="1"/>
     <col min="14086" max="14336" width="10" style="1"/>
-    <col min="14337" max="14337" width="16.140625" style="1" customWidth="1"/>
+    <col min="14337" max="14337" width="16.1796875" style="1" customWidth="1"/>
     <col min="14338" max="14339" width="10" style="1"/>
-    <col min="14340" max="14340" width="14.42578125" style="1" customWidth="1"/>
-    <col min="14341" max="14341" width="13.42578125" style="1" customWidth="1"/>
+    <col min="14340" max="14340" width="14.453125" style="1" customWidth="1"/>
+    <col min="14341" max="14341" width="13.453125" style="1" customWidth="1"/>
     <col min="14342" max="14592" width="10" style="1"/>
-    <col min="14593" max="14593" width="16.140625" style="1" customWidth="1"/>
+    <col min="14593" max="14593" width="16.1796875" style="1" customWidth="1"/>
     <col min="14594" max="14595" width="10" style="1"/>
-    <col min="14596" max="14596" width="14.42578125" style="1" customWidth="1"/>
-    <col min="14597" max="14597" width="13.42578125" style="1" customWidth="1"/>
+    <col min="14596" max="14596" width="14.453125" style="1" customWidth="1"/>
+    <col min="14597" max="14597" width="13.453125" style="1" customWidth="1"/>
     <col min="14598" max="14848" width="10" style="1"/>
-    <col min="14849" max="14849" width="16.140625" style="1" customWidth="1"/>
+    <col min="14849" max="14849" width="16.1796875" style="1" customWidth="1"/>
     <col min="14850" max="14851" width="10" style="1"/>
-    <col min="14852" max="14852" width="14.42578125" style="1" customWidth="1"/>
-    <col min="14853" max="14853" width="13.42578125" style="1" customWidth="1"/>
+    <col min="14852" max="14852" width="14.453125" style="1" customWidth="1"/>
+    <col min="14853" max="14853" width="13.453125" style="1" customWidth="1"/>
     <col min="14854" max="15104" width="10" style="1"/>
-    <col min="15105" max="15105" width="16.140625" style="1" customWidth="1"/>
+    <col min="15105" max="15105" width="16.1796875" style="1" customWidth="1"/>
     <col min="15106" max="15107" width="10" style="1"/>
-    <col min="15108" max="15108" width="14.42578125" style="1" customWidth="1"/>
-    <col min="15109" max="15109" width="13.42578125" style="1" customWidth="1"/>
+    <col min="15108" max="15108" width="14.453125" style="1" customWidth="1"/>
+    <col min="15109" max="15109" width="13.453125" style="1" customWidth="1"/>
     <col min="15110" max="15360" width="10" style="1"/>
-    <col min="15361" max="15361" width="16.140625" style="1" customWidth="1"/>
+    <col min="15361" max="15361" width="16.1796875" style="1" customWidth="1"/>
     <col min="15362" max="15363" width="10" style="1"/>
-    <col min="15364" max="15364" width="14.42578125" style="1" customWidth="1"/>
-    <col min="15365" max="15365" width="13.42578125" style="1" customWidth="1"/>
+    <col min="15364" max="15364" width="14.453125" style="1" customWidth="1"/>
+    <col min="15365" max="15365" width="13.453125" style="1" customWidth="1"/>
     <col min="15366" max="15616" width="10" style="1"/>
-    <col min="15617" max="15617" width="16.140625" style="1" customWidth="1"/>
+    <col min="15617" max="15617" width="16.1796875" style="1" customWidth="1"/>
     <col min="15618" max="15619" width="10" style="1"/>
-    <col min="15620" max="15620" width="14.42578125" style="1" customWidth="1"/>
-    <col min="15621" max="15621" width="13.42578125" style="1" customWidth="1"/>
+    <col min="15620" max="15620" width="14.453125" style="1" customWidth="1"/>
+    <col min="15621" max="15621" width="13.453125" style="1" customWidth="1"/>
     <col min="15622" max="15872" width="10" style="1"/>
-    <col min="15873" max="15873" width="16.140625" style="1" customWidth="1"/>
+    <col min="15873" max="15873" width="16.1796875" style="1" customWidth="1"/>
     <col min="15874" max="15875" width="10" style="1"/>
-    <col min="15876" max="15876" width="14.42578125" style="1" customWidth="1"/>
-    <col min="15877" max="15877" width="13.42578125" style="1" customWidth="1"/>
+    <col min="15876" max="15876" width="14.453125" style="1" customWidth="1"/>
+    <col min="15877" max="15877" width="13.453125" style="1" customWidth="1"/>
     <col min="15878" max="16128" width="10" style="1"/>
-    <col min="16129" max="16129" width="16.140625" style="1" customWidth="1"/>
+    <col min="16129" max="16129" width="16.1796875" style="1" customWidth="1"/>
     <col min="16130" max="16131" width="10" style="1"/>
-    <col min="16132" max="16132" width="14.42578125" style="1" customWidth="1"/>
-    <col min="16133" max="16133" width="13.42578125" style="1" customWidth="1"/>
+    <col min="16132" max="16132" width="14.453125" style="1" customWidth="1"/>
+    <col min="16133" max="16133" width="13.453125" style="1" customWidth="1"/>
     <col min="16134" max="16384" width="10" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="10" customFormat="1" ht="15" thickBot="1">
+    <row r="1" spans="1:6" s="10" customFormat="1" ht="15.5" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>370</v>
       </c>

</xml_diff>